<commit_message>
sample prompts that run before the app - can be used for mysql query stuff
</commit_message>
<xml_diff>
--- a/db-railroad-flowchart.xlsx
+++ b/db-railroad-flowchart.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Claud\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1170" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -75,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -213,6 +219,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -233,7 +247,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -280,7 +300,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -327,7 +353,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -374,7 +406,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -421,7 +459,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -468,7 +512,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Right Bracket 29"/>
+        <xdr:cNvPr id="30" name="Right Bracket 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -520,7 +570,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="Straight Arrow Connector 31"/>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="30" idx="1"/>
         </xdr:cNvCxnSpPr>
@@ -569,7 +625,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="35" name="Straight Connector 34"/>
+        <xdr:cNvPr id="35" name="Straight Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="30" idx="0"/>
         </xdr:cNvCxnSpPr>
@@ -600,6 +662,1863 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27447D75-00AB-4FA4-B833-D098A9B18230}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="590549"/>
+          <a:ext cx="1657350" cy="1352551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Query database with</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Information from form:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>departing_date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>departing_time </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>outgoing_station</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>destination station</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94373FEB-1355-4FF2-B801-AD065AB531A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="2419351"/>
+          <a:ext cx="933450" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5290072-C348-441A-9BD5-C76BB782FEC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2028824" y="3048000"/>
+          <a:ext cx="1704975" cy="1476376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Query database with</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Information from form:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>departing_date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>departing_time </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>return_date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>return_time</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>outgoing_station</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>destination station</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Diamond 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE653698-56A7-420E-93C2-9CFED91D32EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4629149" y="1476375"/>
+          <a:ext cx="3000375" cy="2362200"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Are the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> entries valid? Do the dates/times/destinations produce valid queries or empty tabes?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{876886FD-583F-4B69-84F6-1E42BBBFA179}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="1190625"/>
+          <a:ext cx="1543050" cy="1200149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>If no result is found or the entry is invalid, an empty list will be returned and nothing will be displayed in the results page </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0180A103-018F-4FF4-A5E7-ECC4BD664068}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8239125" y="3200400"/>
+          <a:ext cx="1543050" cy="1200149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>If a trip can be arranged with the user presented specifications. Results will display on page with purchase option</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A57A289A-5F57-4C4C-8307-4759FD97A8FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10972800" y="1009650"/>
+          <a:ext cx="2438400" cy="3952875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Insert into passengers table with values from Purchase form:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>fname</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>lname</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>email</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>billing addr</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>credit card</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>--</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>if tickets &gt;1 </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>fname1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>lname1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>email </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(other information is not necessary)  ...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>each entry will:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Update the seats_free count from the seats_free table according for all the segments that the selected trip is to traverse</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Insert into trips table with the trip details and passenger id </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406224</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>97166</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CDB7538-A217-40F5-9F98-09425B3F3345}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="7"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1092024" y="1266825"/>
+          <a:ext cx="955851" cy="1230641"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406224</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>74286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{225C52F7-903E-4EBF-BFD9-4063E4C55F8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="5"/>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1092024" y="2874636"/>
+          <a:ext cx="936800" cy="911552"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>562127</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>26056</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="911698"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBFC0A9C-5925-4643-8721-527524B4FAED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18447215">
+          <a:off x="924358" y="1749800"/>
+          <a:ext cx="911698" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>One way</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>514630</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47344</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="911698" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7418449-65E1-4664-A34F-CA11BB6E78B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2661393">
+          <a:off x="1200430" y="3047719"/>
+          <a:ext cx="911698" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Round trip</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39F529B2-CFDB-49F1-9061-608D748487E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="5" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705225" y="1266825"/>
+          <a:ext cx="923924" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{207D8E5C-35BE-4E96-BEEA-3DDF5D86B097}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="5" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3733799" y="2657475"/>
+          <a:ext cx="895350" cy="1128713"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A5D08B4-C6C2-4DE3-BAC3-1BB26BBDC593}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7629524" y="2657475"/>
+          <a:ext cx="609601" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFB2C78C-B711-466B-8140-14941DBD6ED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="7" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7629524" y="1790700"/>
+          <a:ext cx="600076" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9ED4241-8483-437F-A105-E71572836917}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9782175" y="2986088"/>
+          <a:ext cx="1190625" cy="814387"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Arrow Connector 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85F24E3-8163-480B-A024-24BC14D877FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9001125" y="209550"/>
+          <a:ext cx="19050" cy="981075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49DC6195-983B-4843-A29C-2864AC81EE44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="695325" y="228600"/>
+          <a:ext cx="8324850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07B8B74-4D99-4E5A-9D00-B82C6DF43163}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="762000" y="238125"/>
+          <a:ext cx="9525" cy="2181226"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>261808</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127124</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="870558" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="TextBox 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{259161E4-DFD8-4F70-9CB0-12C749C52890}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19285961">
+          <a:off x="9863008" y="3127499"/>
+          <a:ext cx="870558" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Purchase</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>293474</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>144676</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="870558"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="TextBox 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088262FA-A9BF-41ED-9DC6-5368A91B7C4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18389483">
+          <a:off x="7534275" y="1847850"/>
+          <a:ext cx="870558" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="870558"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="TextBox 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45E7D12A-5102-407F-A417-CD2372FE9223}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="3729346">
+          <a:off x="7650377" y="3103348"/>
+          <a:ext cx="870558" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -900,18 +2819,26 @@
       </a:style>
     </a:spDef>
     <a:lnDef>
-      <a:spPr/>
+      <a:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </a:spPr>
       <a:bodyPr/>
       <a:lstStyle/>
       <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -927,17 +2854,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="10" max="10" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -949,7 +2876,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -962,7 +2889,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -977,7 +2904,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
@@ -991,7 +2918,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1006,7 +2933,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1023,7 +2950,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1040,7 +2967,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1055,7 +2982,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>0</v>
@@ -1072,7 +2999,7 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="2"/>
       <c r="C10" s="6"/>
@@ -1087,7 +3014,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="2"/>
       <c r="C11" s="6"/>
@@ -1102,7 +3029,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6"/>
@@ -1117,7 +3044,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="45">
+    <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1132,7 +3059,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1145,7 +3072,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1160,7 +3087,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1175,7 +3102,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1190,7 +3117,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1205,7 +3132,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1220,7 +3147,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1235,7 +3162,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1250,7 +3177,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1263,7 +3190,7 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1276,7 +3203,7 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1289,7 +3216,7 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1302,7 +3229,7 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1315,7 +3242,7 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1328,7 +3255,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1341,7 +3268,7 @@
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1354,7 +3281,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1367,7 +3294,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1380,7 +3307,7 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1393,26 +3320,26 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1428,4 +3355,870 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>